<commit_message>
trungdt up code thong ke
</commit_message>
<xml_diff>
--- a/PhanMemQuanLyBanQuanAo/ThongKeSanPham.xlsx
+++ b/PhanMemQuanLyBanQuanAo/ThongKeSanPham.xlsx
@@ -6,18 +6,39 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Thống kê ngày 2022-12-09 2022-1" r:id="rId3" sheetId="1"/>
+    <sheet name="Thống kê ngày 2022-12-04 2022-1" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
-    <t>MaSP</t>
+    <t>SP0001</t>
   </si>
   <si>
-    <t>SP0001</t>
+    <t>Quần Jean</t>
+  </si>
+  <si>
+    <t>Quần</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Đen</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>SP0003</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>SP0004</t>
   </si>
   <si>
     <t>Áo Phông</t>
@@ -26,25 +47,13 @@
     <t>Áo</t>
   </si>
   <si>
-    <t>Xanh</t>
+    <t>M</t>
   </si>
   <si>
-    <t>L</t>
+    <t>Trắng</t>
   </si>
   <si>
-    <t>Da</t>
-  </si>
-  <si>
-    <t>SP0003</t>
-  </si>
-  <si>
-    <t>Áo gió</t>
-  </si>
-  <si>
-    <t>SP0002</t>
-  </si>
-  <si>
-    <t>Áo Khoác</t>
+    <t>Cotton</t>
   </si>
 </sst>
 </file>
@@ -100,25 +109,25 @@
         <v>1.0</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="n">
-        <v>188.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="2">
@@ -126,25 +135,25 @@
         <v>2.0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
       <c r="H2" t="n">
-        <v>999.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -152,25 +161,25 @@
         <v>3.0</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H3" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>